<commit_message>
Perbaikan error di rekap realisasi per timja
</commit_message>
<xml_diff>
--- a/Database/Cetak Monitoring Perintah Bayar.xlsx
+++ b/Database/Cetak Monitoring Perintah Bayar.xlsx
@@ -211,27 +211,36 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">BELUM DIBUAT KUITANSI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BELUM DIBUAT DRPP</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BELUM DIBUAT SPP</t>
+      <t xml:space="preserve">00032/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00005/DRPP/626402/202
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00049T</t>
     </r>
   </si>
   <si>
@@ -251,6 +260,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00031/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00030/PB/626402/2024</t>
     </r>
   </si>
@@ -261,6 +280,35 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00030/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00004/DRPP/626402/202
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00029/PB/626402/2024</t>
     </r>
   </si>
@@ -271,6 +319,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00029/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00028/PB/626402/2024</t>
     </r>
   </si>
@@ -281,6 +339,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00028/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00027/PB/626402/2024</t>
     </r>
   </si>
@@ -291,6 +359,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00027/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00026/PB/626402/2024</t>
     </r>
   </si>
@@ -301,6 +379,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00026/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00025/PB/626402/2024</t>
     </r>
   </si>
@@ -311,6 +399,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00025/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00024/PB/626402/2024</t>
     </r>
   </si>
@@ -321,6 +419,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00024/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00023/PB/626402/2024</t>
     </r>
   </si>
@@ -331,6 +439,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00023/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00022/PB/626402/2024</t>
     </r>
   </si>
@@ -341,6 +459,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00022/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00021/PB/626402/2024</t>
     </r>
   </si>
@@ -351,6 +479,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00021/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00020/PB/626402/2024</t>
     </r>
   </si>
@@ -361,6 +499,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00020/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00019/PB/626402/2024</t>
     </r>
   </si>
@@ -371,6 +519,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00019/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00018/PB/626402/2024</t>
     </r>
   </si>
@@ -381,6 +539,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00018/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00017/PB/626402/2024</t>
     </r>
   </si>
@@ -391,6 +559,35 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00017/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00002/DRPP/626402/202
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00016/PB/626402/2024</t>
     </r>
   </si>
@@ -401,6 +598,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00016/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00015/PB/626402/2024</t>
     </r>
   </si>
@@ -411,12 +618,51 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00015/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00001/DRPP/626402/202
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00014/PB/626402/2024</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00014/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="10.0"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -441,6 +687,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00013/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00012/PB/626402/2024</t>
     </r>
   </si>
@@ -451,6 +707,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00012/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00011/PB/626402/2024</t>
     </r>
   </si>
@@ -461,6 +727,35 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00011/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00003/DRPP/626402/202
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00010/PB/626402/2024</t>
     </r>
   </si>
@@ -471,6 +766,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00010/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00009/PB/626402/2024</t>
     </r>
   </si>
@@ -481,6 +786,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00009/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00008/PB/626402/2024</t>
     </r>
   </si>
@@ -491,6 +806,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00008/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00007/PB/626402/2024</t>
     </r>
   </si>
@@ -501,6 +826,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00007/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00006/PB/626402/2024</t>
     </r>
   </si>
@@ -511,6 +846,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00006/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00005/PB/626402/2024</t>
     </r>
   </si>
@@ -521,6 +866,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00005/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00004/PB/626402/2024</t>
     </r>
   </si>
@@ -531,6 +886,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00004/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00003/PB/626402/2024</t>
     </r>
   </si>
@@ -541,6 +906,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00003/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00002/PB/626402/2024</t>
     </r>
   </si>
@@ -551,7 +926,27 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">00002/KW/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">00001/PB/626402/2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8.0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00001/KW/626402/2024</t>
     </r>
   </si>
 </sst>
@@ -625,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fillId="0" borderId="0" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -658,6 +1053,9 @@
     </xf>
     <xf numFmtId="0" fillId="0" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fillId="0" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fillId="0" borderId="0" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="101" wrapText="1"/>
@@ -1101,7 +1499,7 @@
       </c>
       <c r="M6" s="0"/>
     </row>
-    <row r="7" spans="1:13" ht="21.00" customHeight="1">
+    <row r="7" spans="1:13" ht="22.50" customHeight="1">
       <c r="A7" s="7">
         <v>45313.000000</v>
       </c>
@@ -1118,7 +1516,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="10"/>
@@ -1130,7 +1528,7 @@
       </c>
       <c r="M7" s="0"/>
     </row>
-    <row r="8" spans="1:13" ht="20.00" customHeight="1">
+    <row r="8" spans="1:13" ht="22.50" customHeight="1">
       <c r="A8" s="7">
         <v>45311.000000</v>
       </c>
@@ -1144,10 +1542,10 @@
         <v>8080980.00</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="10"/>
@@ -1159,12 +1557,12 @@
       </c>
       <c r="M8" s="0"/>
     </row>
-    <row r="9" spans="1:13" ht="20.00" customHeight="1">
+    <row r="9" spans="1:13" ht="22.50" customHeight="1">
       <c r="A9" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="8">
         <v>524119</v>
@@ -1173,11 +1571,11 @@
         <v>3849000.00</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
+      <c r="G9" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -1188,12 +1586,12 @@
       </c>
       <c r="M9" s="0"/>
     </row>
-    <row r="10" spans="1:13" ht="20.00" customHeight="1">
+    <row r="10" spans="1:13" ht="22.50" customHeight="1">
       <c r="A10" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8">
         <v>524119</v>
@@ -1202,11 +1600,11 @@
         <v>2500000.00</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="4" t="s">
-        <v>19</v>
+      <c r="G10" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1217,12 +1615,12 @@
       </c>
       <c r="M10" s="0"/>
     </row>
-    <row r="11" spans="1:13" ht="20.00" customHeight="1">
+    <row r="11" spans="1:13" ht="22.50" customHeight="1">
       <c r="A11" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8">
         <v>524119</v>
@@ -1231,11 +1629,11 @@
         <v>6459556.00</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="4" t="s">
-        <v>19</v>
+      <c r="G11" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -1246,12 +1644,12 @@
       </c>
       <c r="M11" s="0"/>
     </row>
-    <row r="12" spans="1:13" ht="20.00" customHeight="1">
+    <row r="12" spans="1:13" ht="22.50" customHeight="1">
       <c r="A12" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8">
         <v>524119</v>
@@ -1260,11 +1658,11 @@
         <v>3770747.00</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="4" t="s">
-        <v>19</v>
+      <c r="G12" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1275,12 +1673,12 @@
       </c>
       <c r="M12" s="0"/>
     </row>
-    <row r="13" spans="1:13" ht="20.00" customHeight="1">
+    <row r="13" spans="1:13" ht="22.50" customHeight="1">
       <c r="A13" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" s="8">
         <v>524119</v>
@@ -1289,11 +1687,11 @@
         <v>1259500.00</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="4" t="s">
-        <v>19</v>
+      <c r="G13" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -1304,12 +1702,12 @@
       </c>
       <c r="M13" s="0"/>
     </row>
-    <row r="14" spans="1:13" ht="20.00" customHeight="1">
+    <row r="14" spans="1:13" ht="22.50" customHeight="1">
       <c r="A14" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8">
         <v>524119</v>
@@ -1318,11 +1716,11 @@
         <v>1250000.00</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="4" t="s">
-        <v>19</v>
+      <c r="G14" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1333,12 +1731,12 @@
       </c>
       <c r="M14" s="0"/>
     </row>
-    <row r="15" spans="1:13" ht="20.00" customHeight="1">
+    <row r="15" spans="1:13" ht="22.50" customHeight="1">
       <c r="A15" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C15" s="8">
         <v>524119</v>
@@ -1347,11 +1745,11 @@
         <v>4410646.00</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="4" t="s">
-        <v>19</v>
+      <c r="G15" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1362,12 +1760,12 @@
       </c>
       <c r="M15" s="0"/>
     </row>
-    <row r="16" spans="1:13" ht="20.00" customHeight="1">
+    <row r="16" spans="1:13" ht="22.50" customHeight="1">
       <c r="A16" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C16" s="8">
         <v>524119</v>
@@ -1376,11 +1774,11 @@
         <v>3264380.00</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="4" t="s">
-        <v>19</v>
+      <c r="G16" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1391,12 +1789,12 @@
       </c>
       <c r="M16" s="0"/>
     </row>
-    <row r="17" spans="1:13" ht="20.00" customHeight="1">
+    <row r="17" spans="1:13" ht="22.50" customHeight="1">
       <c r="A17" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C17" s="8">
         <v>524119</v>
@@ -1405,11 +1803,11 @@
         <v>1587000.00</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="4" t="s">
-        <v>19</v>
+      <c r="G17" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1420,12 +1818,12 @@
       </c>
       <c r="M17" s="0"/>
     </row>
-    <row r="18" spans="1:13" ht="20.00" customHeight="1">
+    <row r="18" spans="1:13" ht="22.50" customHeight="1">
       <c r="A18" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C18" s="8">
         <v>524119</v>
@@ -1434,11 +1832,11 @@
         <v>6148000.00</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F18" s="10"/>
-      <c r="G18" s="4" t="s">
-        <v>19</v>
+      <c r="G18" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1449,12 +1847,12 @@
       </c>
       <c r="M18" s="0"/>
     </row>
-    <row r="19" spans="1:13" ht="20.00" customHeight="1">
+    <row r="19" spans="1:13" ht="22.50" customHeight="1">
       <c r="A19" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8">
         <v>524119</v>
@@ -1463,11 +1861,11 @@
         <v>4968155.00</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="4" t="s">
-        <v>19</v>
+      <c r="G19" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1478,12 +1876,12 @@
       </c>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" spans="1:13" ht="20.00" customHeight="1">
+    <row r="20" spans="1:13" ht="22.50" customHeight="1">
       <c r="A20" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8">
         <v>524119</v>
@@ -1492,11 +1890,11 @@
         <v>2297400.00</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F20" s="10"/>
-      <c r="G20" s="4" t="s">
-        <v>19</v>
+      <c r="G20" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1507,12 +1905,12 @@
       </c>
       <c r="M20" s="0"/>
     </row>
-    <row r="21" spans="1:13" ht="20.00" customHeight="1">
+    <row r="21" spans="1:13" ht="22.50" customHeight="1">
       <c r="A21" s="7">
         <v>45309.000000</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C21" s="8">
         <v>524119</v>
@@ -1521,11 +1919,11 @@
         <v>1250000.00</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F21" s="10"/>
-      <c r="G21" s="4" t="s">
-        <v>19</v>
+      <c r="G21" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -1536,12 +1934,12 @@
       </c>
       <c r="M21" s="0"/>
     </row>
-    <row r="22" spans="1:13" ht="20.00" customHeight="1">
+    <row r="22" spans="1:13" ht="22.50" customHeight="1">
       <c r="A22" s="7">
         <v>45313.000000</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8">
         <v>524111</v>
@@ -1550,11 +1948,11 @@
         <v>5285500.00</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F22" s="10"/>
-      <c r="G22" s="4" t="s">
-        <v>19</v>
+      <c r="G22" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
@@ -1565,12 +1963,12 @@
       </c>
       <c r="M22" s="0"/>
     </row>
-    <row r="23" spans="1:13" ht="20.00" customHeight="1">
+    <row r="23" spans="1:13" ht="22.50" customHeight="1">
       <c r="A23" s="7">
         <v>45313.000000</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C23" s="8">
         <v>524111</v>
@@ -1579,11 +1977,11 @@
         <v>6756655.00</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="4" t="s">
-        <v>19</v>
+      <c r="G23" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -1594,12 +1992,12 @@
       </c>
       <c r="M23" s="0"/>
     </row>
-    <row r="24" spans="1:13" ht="20.00" customHeight="1">
+    <row r="24" spans="1:13" ht="22.50" customHeight="1">
       <c r="A24" s="7">
         <v>45306.000000</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C24" s="8">
         <v>524111</v>
@@ -1608,11 +2006,11 @@
         <v>6269025.00</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="F24" s="10"/>
-      <c r="G24" s="4" t="s">
-        <v>19</v>
+      <c r="G24" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -1623,12 +2021,12 @@
       </c>
       <c r="M24" s="0"/>
     </row>
-    <row r="25" spans="1:13" ht="20.00" customHeight="1">
+    <row r="25" spans="1:13" ht="22.50" customHeight="1">
       <c r="A25" s="7">
         <v>45306.000000</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C25" s="8">
         <v>524111</v>
@@ -1637,11 +2035,11 @@
         <v>2132100.00</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="4" t="s">
-        <v>19</v>
+      <c r="G25" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
@@ -1653,21 +2051,21 @@
       <c r="M25" s="0"/>
     </row>
     <row r="26" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="A26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
     </row>
     <row r="27" spans="1:13" ht="25.00" customHeight="1">
       <c r="A27" s="4" t="s">
@@ -1708,12 +2106,12 @@
       </c>
       <c r="M27" s="0"/>
     </row>
-    <row r="28" spans="1:13" ht="20.00" customHeight="1">
+    <row r="28" spans="1:13" ht="22.50" customHeight="1">
       <c r="A28" s="7">
         <v>45301.000000</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C28" s="8">
         <v>524111</v>
@@ -1722,11 +2120,11 @@
         <v>2304000.00</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F28" s="10"/>
-      <c r="G28" s="4" t="s">
-        <v>19</v>
+      <c r="G28" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -1737,12 +2135,12 @@
       </c>
       <c r="M28" s="0"/>
     </row>
-    <row r="29" spans="1:13" ht="20.00" customHeight="1">
+    <row r="29" spans="1:13" ht="22.50" customHeight="1">
       <c r="A29" s="7">
         <v>45301.000000</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C29" s="8">
         <v>524111</v>
@@ -1751,11 +2149,11 @@
         <v>3772929.00</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="F29" s="10"/>
-      <c r="G29" s="4" t="s">
-        <v>19</v>
+      <c r="G29" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -1766,12 +2164,12 @@
       </c>
       <c r="M29" s="0"/>
     </row>
-    <row r="30" spans="1:13" ht="20.00" customHeight="1">
+    <row r="30" spans="1:13" ht="22.50" customHeight="1">
       <c r="A30" s="7">
         <v>45310.000000</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C30" s="8">
         <v>524111</v>
@@ -1780,11 +2178,11 @@
         <v>600000.00</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F30" s="10"/>
-      <c r="G30" s="4" t="s">
-        <v>19</v>
+      <c r="G30" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -1795,12 +2193,12 @@
       </c>
       <c r="M30" s="0"/>
     </row>
-    <row r="31" spans="1:13" ht="20.00" customHeight="1">
+    <row r="31" spans="1:13" ht="22.50" customHeight="1">
       <c r="A31" s="7">
         <v>45305.000000</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C31" s="8">
         <v>524111</v>
@@ -1809,11 +2207,11 @@
         <v>3351000.00</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="F31" s="10"/>
-      <c r="G31" s="4" t="s">
-        <v>19</v>
+      <c r="G31" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
@@ -1824,12 +2222,12 @@
       </c>
       <c r="M31" s="0"/>
     </row>
-    <row r="32" spans="1:13" ht="20.00" customHeight="1">
+    <row r="32" spans="1:13" ht="22.50" customHeight="1">
       <c r="A32" s="7">
         <v>45305.000000</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C32" s="8">
         <v>524111</v>
@@ -1838,11 +2236,11 @@
         <v>2398000.00</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="F32" s="10"/>
-      <c r="G32" s="4" t="s">
-        <v>19</v>
+      <c r="G32" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -1853,12 +2251,12 @@
       </c>
       <c r="M32" s="0"/>
     </row>
-    <row r="33" spans="1:13" ht="20.00" customHeight="1">
+    <row r="33" spans="1:13" ht="22.50" customHeight="1">
       <c r="A33" s="7">
         <v>45294.000000</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C33" s="8">
         <v>524111</v>
@@ -1867,11 +2265,11 @@
         <v>651500.00</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="F33" s="10"/>
-      <c r="G33" s="4" t="s">
-        <v>19</v>
+      <c r="G33" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -1882,12 +2280,12 @@
       </c>
       <c r="M33" s="0"/>
     </row>
-    <row r="34" spans="1:13" ht="20.00" customHeight="1">
+    <row r="34" spans="1:13" ht="22.50" customHeight="1">
       <c r="A34" s="7">
         <v>45312.000000</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C34" s="8">
         <v>521219</v>
@@ -1896,11 +2294,11 @@
         <v>1615470.00</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="F34" s="10"/>
-      <c r="G34" s="4" t="s">
-        <v>19</v>
+      <c r="G34" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
@@ -1911,12 +2309,12 @@
       </c>
       <c r="M34" s="0"/>
     </row>
-    <row r="35" spans="1:13" ht="20.00" customHeight="1">
+    <row r="35" spans="1:13" ht="22.50" customHeight="1">
       <c r="A35" s="7">
         <v>45310.000000</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C35" s="8">
         <v>521211</v>
@@ -1925,11 +2323,11 @@
         <v>810000.00</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F35" s="10"/>
-      <c r="G35" s="4" t="s">
-        <v>19</v>
+      <c r="G35" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
@@ -1940,12 +2338,12 @@
       </c>
       <c r="M35" s="0"/>
     </row>
-    <row r="36" spans="1:13" ht="20.00" customHeight="1">
+    <row r="36" spans="1:13" ht="22.50" customHeight="1">
       <c r="A36" s="7">
         <v>45306.000000</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C36" s="8">
         <v>521211</v>
@@ -1954,11 +2352,11 @@
         <v>1270500.00</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F36" s="10"/>
-      <c r="G36" s="4" t="s">
-        <v>19</v>
+      <c r="G36" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
@@ -1969,12 +2367,12 @@
       </c>
       <c r="M36" s="0"/>
     </row>
-    <row r="37" spans="1:13" ht="20.00" customHeight="1">
+    <row r="37" spans="1:13" ht="22.50" customHeight="1">
       <c r="A37" s="7">
         <v>45306.000000</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="C37" s="8">
         <v>521211</v>
@@ -1983,11 +2381,11 @@
         <v>660000.00</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="F37" s="10"/>
-      <c r="G37" s="4" t="s">
-        <v>19</v>
+      <c r="G37" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
@@ -1998,12 +2396,12 @@
       </c>
       <c r="M37" s="0"/>
     </row>
-    <row r="38" spans="1:13" ht="20.00" customHeight="1">
+    <row r="38" spans="1:13" ht="22.50" customHeight="1">
       <c r="A38" s="7">
         <v>45301.000000</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C38" s="8">
         <v>524111</v>
@@ -2012,11 +2410,11 @@
         <v>818500.00</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="F38" s="10"/>
-      <c r="G38" s="4" t="s">
-        <v>19</v>
+      <c r="G38" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -2027,12 +2425,12 @@
       </c>
       <c r="M38" s="0"/>
     </row>
-    <row r="39" spans="1:13" ht="20.00" customHeight="1">
+    <row r="39" spans="1:13" ht="22.50" customHeight="1">
       <c r="A39" s="7">
         <v>45295.000000</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C39" s="8">
         <v>521211</v>
@@ -2041,11 +2439,11 @@
         <v>1060000.00</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="F39" s="10"/>
-      <c r="G39" s="4" t="s">
-        <v>19</v>
+      <c r="G39" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -2056,12 +2454,12 @@
       </c>
       <c r="M39" s="0"/>
     </row>
-    <row r="40" spans="1:13" ht="20.00" customHeight="1">
+    <row r="40" spans="1:13" ht="22.50" customHeight="1">
       <c r="A40" s="7">
         <v>45295.000000</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C40" s="8">
         <v>521211</v>
@@ -2070,11 +2468,11 @@
         <v>440000.00</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="F40" s="10"/>
-      <c r="G40" s="4" t="s">
-        <v>19</v>
+      <c r="G40" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>

</xml_diff>